<commit_message>
mean anomaly uranus moons
</commit_message>
<xml_diff>
--- a/src/app/scene/data/uranus.xlsx
+++ b/src/app/scene/data/uranus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl03940s\Documents\GitHub\solar-system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl03940s\Documents\GitHub\solar-system\src\app\scene\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="109">
   <si>
     <t>Order</t>
   </si>
@@ -326,12 +326,96 @@
   <si>
     <t>Margaret</t>
   </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>254.8</t>
+  </si>
+  <si>
+    <t>116.3</t>
+  </si>
+  <si>
+    <t>138.5</t>
+  </si>
+  <si>
+    <t>233.8</t>
+  </si>
+  <si>
+    <t>184.6</t>
+  </si>
+  <si>
+    <t>244.7</t>
+  </si>
+  <si>
+    <t>218.3</t>
+  </si>
+  <si>
+    <t>136.1</t>
+  </si>
+  <si>
+    <t>163.8</t>
+  </si>
+  <si>
+    <t>357.2</t>
+  </si>
+  <si>
+    <t>192.4</t>
+  </si>
+  <si>
+    <t>245.8</t>
+  </si>
+  <si>
+    <t>273.8</t>
+  </si>
+  <si>
+    <t>311.3</t>
+  </si>
+  <si>
+    <t>39.5</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>24.6</t>
+  </si>
+  <si>
+    <t>283.1</t>
+  </si>
+  <si>
+    <t>90.9</t>
+  </si>
+  <si>
+    <t>163.5</t>
+  </si>
+  <si>
+    <t>188.1</t>
+  </si>
+  <si>
+    <t>194.9</t>
+  </si>
+  <si>
+    <t>260.9</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>316.8</t>
+  </si>
+  <si>
+    <t>247.6</t>
+  </si>
+  <si>
+    <t>216.4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,6 +470,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF888888"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF00FF"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -480,7 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -524,13 +632,25 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -815,7 +935,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L3" sqref="L3:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +944,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -844,7 +964,7 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
@@ -856,6 +976,9 @@
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>81</v>
       </c>
       <c r="H2" t="s">
         <v>49</v>
@@ -892,6 +1015,9 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="G3" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="H3" t="str">
         <f>UPPER(SUBSTITUTE(SUBSTITUTE(B3," ","_"),"/","_"))</f>
         <v>CORDELIA</v>
@@ -900,7 +1026,7 @@
         <f>LOWER(SUBSTITUTE(SUBSTITUTE(B3," ","-"),"/","/"))</f>
         <v>cordelia</v>
       </c>
-      <c r="J3" s="17" t="str">
+      <c r="J3" s="15" t="str">
         <f>SUBSTITUTE(C3/2,",",".")</f>
         <v>20</v>
       </c>
@@ -921,7 +1047,7 @@
   semiMajorAxis: "&amp;E3&amp;",
   eccentricity: "&amp;F3&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G3&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -939,7 +1065,7 @@
   semiMajorAxis: 49770,
   eccentricity: 0.00026,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 254.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -966,6 +1092,9 @@
       <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="G4" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="H4" t="str">
         <f t="shared" ref="H4:H29" si="0">UPPER(SUBSTITUTE(SUBSTITUTE(B4," ","_"),"/","_"))</f>
         <v>OPHELIA</v>
@@ -974,7 +1103,7 @@
         <f t="shared" ref="I4:I29" si="1">LOWER(SUBSTITUTE(SUBSTITUTE(B4," ","-"),"/","/"))</f>
         <v>ophelia</v>
       </c>
-      <c r="J4" s="17" t="str">
+      <c r="J4" s="15" t="str">
         <f t="shared" ref="J4:J29" si="2">SUBSTITUTE(C4/2,",",".")</f>
         <v>21.5</v>
       </c>
@@ -995,7 +1124,7 @@
   semiMajorAxis: "&amp;E4&amp;",
   eccentricity: "&amp;F4&amp;",
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: "&amp;G4&amp;",
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1013,7 +1142,7 @@
   semiMajorAxis: 53790,
   eccentricity: 0.00992,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 116.3,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1040,6 +1169,9 @@
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G5" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>BIANCA</v>
@@ -1048,7 +1180,7 @@
         <f t="shared" si="1"/>
         <v>bianca</v>
       </c>
-      <c r="J5" s="17" t="str">
+      <c r="J5" s="15" t="str">
         <f t="shared" si="2"/>
         <v>25.5</v>
       </c>
@@ -1070,7 +1202,7 @@
   semiMajorAxis: 59170,
   eccentricity: 0.00092,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 138.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1097,6 +1229,9 @@
       <c r="F6" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="G6" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>CRESSIDA</v>
@@ -1105,7 +1240,7 @@
         <f t="shared" si="1"/>
         <v>cressida</v>
       </c>
-      <c r="J6" s="17" t="str">
+      <c r="J6" s="15" t="str">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -1127,7 +1262,7 @@
   semiMajorAxis: 61780,
   eccentricity: 0.00036,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 233.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1154,6 +1289,9 @@
       <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="G7" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>DESDEMONA</v>
@@ -1162,7 +1300,7 @@
         <f t="shared" si="1"/>
         <v>desdemona</v>
       </c>
-      <c r="J7" s="17" t="str">
+      <c r="J7" s="15" t="str">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
@@ -1184,7 +1322,7 @@
   semiMajorAxis: 62680,
   eccentricity: 0.00013,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 184.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1211,6 +1349,9 @@
       <c r="F8" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="G8" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
         <v>JULIET</v>
@@ -1219,7 +1360,7 @@
         <f t="shared" si="1"/>
         <v>juliet</v>
       </c>
-      <c r="J8" s="17" t="str">
+      <c r="J8" s="15" t="str">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
@@ -1241,7 +1382,7 @@
   semiMajorAxis: 64350,
   eccentricity: 0.00066,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 244.7,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1268,6 +1409,9 @@
       <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="G9" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
         <v>PORTIA</v>
@@ -1276,7 +1420,7 @@
         <f t="shared" si="1"/>
         <v>portia</v>
       </c>
-      <c r="J9" s="17" t="str">
+      <c r="J9" s="15" t="str">
         <f t="shared" si="2"/>
         <v>67.5</v>
       </c>
@@ -1298,7 +1442,7 @@
   semiMajorAxis: 66090,
   eccentricity: 0.00005,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 218.3,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1325,6 +1469,9 @@
       <c r="F10" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="G10" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
         <v>ROSALIND</v>
@@ -1333,7 +1480,7 @@
         <f t="shared" si="1"/>
         <v>rosalind</v>
       </c>
-      <c r="J10" s="17" t="str">
+      <c r="J10" s="15" t="str">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -1355,7 +1502,7 @@
   semiMajorAxis: 69940,
   eccentricity: 0.00011,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 136.1,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1382,6 +1529,9 @@
       <c r="F11" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="G11" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
         <v>CUPID</v>
@@ -1390,7 +1540,7 @@
         <f t="shared" si="1"/>
         <v>cupid</v>
       </c>
-      <c r="J11" s="17" t="str">
+      <c r="J11" s="15" t="str">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -1412,7 +1562,7 @@
   semiMajorAxis: 74800,
   eccentricity: 0.0013,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 163.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1439,6 +1589,9 @@
       <c r="F12" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="G12" s="18" t="s">
+        <v>91</v>
+      </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
         <v>BELINDA</v>
@@ -1447,7 +1600,7 @@
         <f t="shared" si="1"/>
         <v>belinda</v>
       </c>
-      <c r="J12" s="17" t="str">
+      <c r="J12" s="15" t="str">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -1469,7 +1622,7 @@
   semiMajorAxis: 75260,
   eccentricity: 0.00007,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 357.2,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1496,6 +1649,9 @@
       <c r="F13" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="G13" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
         <v>PERDITA</v>
@@ -1504,7 +1660,7 @@
         <f t="shared" si="1"/>
         <v>perdita</v>
       </c>
-      <c r="J13" s="17" t="str">
+      <c r="J13" s="15" t="str">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -1526,7 +1682,7 @@
   semiMajorAxis: 76400,
   eccentricity: 0.0012,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 192.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1553,6 +1709,9 @@
       <c r="F14" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="G14" s="18" t="s">
+        <v>93</v>
+      </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
         <v>PUCK</v>
@@ -1561,7 +1720,7 @@
         <f t="shared" si="1"/>
         <v>puck</v>
       </c>
-      <c r="J14" s="17" t="str">
+      <c r="J14" s="15" t="str">
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
@@ -1583,7 +1742,7 @@
   semiMajorAxis: 86010,
   eccentricity: 0.00012,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 245.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1610,6 +1769,9 @@
       <c r="F15" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="G15" s="18" t="s">
+        <v>94</v>
+      </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
         <v>MAB</v>
@@ -1618,7 +1780,7 @@
         <f t="shared" si="1"/>
         <v>mab</v>
       </c>
-      <c r="J15" s="17" t="str">
+      <c r="J15" s="15" t="str">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
@@ -1640,7 +1802,7 @@
   semiMajorAxis: 97700,
   eccentricity: 0.0025,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 273.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1667,6 +1829,9 @@
       <c r="F16" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="G16" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
         <v>MIRANDA</v>
@@ -1675,7 +1840,7 @@
         <f t="shared" si="1"/>
         <v>miranda</v>
       </c>
-      <c r="J16" s="17" t="str">
+      <c r="J16" s="15" t="str">
         <f t="shared" si="2"/>
         <v>235.8</v>
       </c>
@@ -1697,7 +1862,7 @@
   semiMajorAxis: 129390,
   eccentricity: 0.0013,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 311.3,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1724,6 +1889,9 @@
       <c r="F17" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="G17" s="19" t="s">
+        <v>96</v>
+      </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
         <v>ARIEL</v>
@@ -1732,7 +1900,7 @@
         <f t="shared" si="1"/>
         <v>ariel</v>
       </c>
-      <c r="J17" s="17" t="str">
+      <c r="J17" s="15" t="str">
         <f t="shared" si="2"/>
         <v>578.9</v>
       </c>
@@ -1754,7 +1922,7 @@
   semiMajorAxis: 191020,
   eccentricity: 0.0012,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 39.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1781,6 +1949,9 @@
       <c r="F18" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="G18" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
         <v>UMBRIEL</v>
@@ -1789,7 +1960,7 @@
         <f t="shared" si="1"/>
         <v>umbriel</v>
       </c>
-      <c r="J18" s="17" t="str">
+      <c r="J18" s="15" t="str">
         <f t="shared" si="2"/>
         <v>584.7</v>
       </c>
@@ -1811,7 +1982,7 @@
   semiMajorAxis: 266300,
   eccentricity: 0.0039,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 12.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1838,6 +2009,9 @@
       <c r="F19" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="G19" s="19" t="s">
+        <v>98</v>
+      </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
         <v>TITANIA</v>
@@ -1846,7 +2020,7 @@
         <f t="shared" si="1"/>
         <v>titania</v>
       </c>
-      <c r="J19" s="17" t="str">
+      <c r="J19" s="15" t="str">
         <f t="shared" si="2"/>
         <v>788.4</v>
       </c>
@@ -1868,7 +2042,7 @@
   semiMajorAxis: 435910,
   eccentricity: 0.0011,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 24.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1895,6 +2069,9 @@
       <c r="F20" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="G20" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
         <v>OBERON</v>
@@ -1903,7 +2080,7 @@
         <f t="shared" si="1"/>
         <v>oberon</v>
       </c>
-      <c r="J20" s="17" t="str">
+      <c r="J20" s="15" t="str">
         <f t="shared" si="2"/>
         <v>761.4</v>
       </c>
@@ -1925,7 +2102,7 @@
   semiMajorAxis: 583520,
   eccentricity: 0.0014,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 283.1,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -1952,6 +2129,9 @@
       <c r="F21" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="G21" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
         <v>FRANCISCO</v>
@@ -1960,7 +2140,7 @@
         <f t="shared" si="1"/>
         <v>francisco</v>
       </c>
-      <c r="J21" s="17" t="str">
+      <c r="J21" s="15" t="str">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -1982,7 +2162,7 @@
   semiMajorAxis: 4282900,
   eccentricity: 0.1324,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 90.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2009,6 +2189,9 @@
       <c r="F22" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="G22" s="20" t="s">
+        <v>101</v>
+      </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
         <v>CALIBAN</v>
@@ -2017,7 +2200,7 @@
         <f t="shared" si="1"/>
         <v>caliban</v>
       </c>
-      <c r="J22" s="17" t="str">
+      <c r="J22" s="15" t="str">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -2039,7 +2222,7 @@
   semiMajorAxis: 7231100,
   eccentricity: 0.1812,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 163.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2066,6 +2249,9 @@
       <c r="F23" s="9" t="s">
         <v>31</v>
       </c>
+      <c r="G23" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
         <v>STEPHANO</v>
@@ -2074,7 +2260,7 @@
         <f t="shared" si="1"/>
         <v>stephano</v>
       </c>
-      <c r="J23" s="17" t="str">
+      <c r="J23" s="15" t="str">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -2096,7 +2282,7 @@
   semiMajorAxis: 8007400,
   eccentricity: 0.2248,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 188.1,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2123,6 +2309,9 @@
       <c r="F24" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="G24" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
         <v>TRINCULO</v>
@@ -2131,7 +2320,7 @@
         <f t="shared" si="1"/>
         <v>trinculo</v>
       </c>
-      <c r="J24" s="17" t="str">
+      <c r="J24" s="15" t="str">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -2153,7 +2342,7 @@
   semiMajorAxis: 8505200,
   eccentricity: 0.2194,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 194.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2180,6 +2369,9 @@
       <c r="F25" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="G25" s="20" t="s">
+        <v>104</v>
+      </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
         <v>SYCORAX</v>
@@ -2188,7 +2380,7 @@
         <f t="shared" si="1"/>
         <v>sycorax</v>
       </c>
-      <c r="J25" s="17" t="str">
+      <c r="J25" s="15" t="str">
         <f t="shared" si="2"/>
         <v>78.5</v>
       </c>
@@ -2210,7 +2402,7 @@
   semiMajorAxis: 12179400,
   eccentricity: 0.5219,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 260.9,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2237,6 +2429,9 @@
       <c r="F26" s="13" t="s">
         <v>34</v>
       </c>
+      <c r="G26" s="21" t="s">
+        <v>105</v>
+      </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
         <v>MARGARET</v>
@@ -2245,7 +2440,7 @@
         <f t="shared" si="1"/>
         <v>margaret</v>
       </c>
-      <c r="J26" s="17" t="str">
+      <c r="J26" s="15" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -2267,7 +2462,7 @@
   semiMajorAxis: 14146700,
   eccentricity: 0.6772,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 3.5,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2294,6 +2489,9 @@
       <c r="F27" s="9" t="s">
         <v>35</v>
       </c>
+      <c r="G27" s="20" t="s">
+        <v>106</v>
+      </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
         <v>PROSPERO</v>
@@ -2302,7 +2500,7 @@
         <f t="shared" si="1"/>
         <v>prospero</v>
       </c>
-      <c r="J27" s="17" t="str">
+      <c r="J27" s="15" t="str">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -2324,7 +2522,7 @@
   semiMajorAxis: 16276800,
   eccentricity: 0.4445,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 316.8,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2351,6 +2549,9 @@
       <c r="F28" s="9" t="s">
         <v>36</v>
       </c>
+      <c r="G28" s="20" t="s">
+        <v>107</v>
+      </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
         <v>SETEBOS</v>
@@ -2359,7 +2560,7 @@
         <f t="shared" si="1"/>
         <v>setebos</v>
       </c>
-      <c r="J28" s="17" t="str">
+      <c r="J28" s="15" t="str">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -2381,7 +2582,7 @@
   semiMajorAxis: 17420400,
   eccentricity: 0.5908,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 247.6,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null
@@ -2408,6 +2609,9 @@
       <c r="F29" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="G29" s="20" t="s">
+        <v>108</v>
+      </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
         <v>FERDINAND</v>
@@ -2416,7 +2620,7 @@
         <f t="shared" si="1"/>
         <v>ferdinand</v>
       </c>
-      <c r="J29" s="17" t="str">
+      <c r="J29" s="15" t="str">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -2438,7 +2642,7 @@
   semiMajorAxis: 20430000,
   eccentricity: 0.3993,
   trueAnomaly: 0,
-  meanAnomaly: 0, // TODO
+  meanAnomaly: 216.4,
   type: CELESTIAL_BODY_TYPE.SATELLITE,
   satellites: [],
   orbitBody: null

</xml_diff>